<commit_message>
correct a small bug
</commit_message>
<xml_diff>
--- a/res/dev/func/test_func.xlsx
+++ b/res/dev/func/test_func.xlsx
@@ -3172,7 +3172,7 @@
     <definedNames>
       <definedName name="MDF"/>
       <definedName name="udf_arrange"/>
-      <definedName name="udf_arrange_mutli"/>
+      <definedName name="udf_arrange_multi"/>
       <definedName name="udf_md5"/>
       <definedName name="udf_md5_single"/>
       <definedName name="udf_sample"/>
@@ -3474,8 +3474,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:R1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3553,7 +3553,7 @@
         <v>1</v>
       </c>
       <c r="Q5" t="str">
-        <f t="array" ref="Q5:R18">[1]!udf_arrange_mutli(N5:N7,O4:P4,O5:P7)</f>
+        <f t="array" ref="Q5:R18">[1]!udf_arrange_multi(N5:N7,O4:P4,O5:P7)</f>
         <v>task1</v>
       </c>
       <c r="R5" t="str">
@@ -4452,7 +4452,7 @@
         <v>1</v>
       </c>
       <c r="E58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.15">
@@ -5418,7 +5418,7 @@
         <v>1</v>
       </c>
       <c r="E127" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="2:5" x14ac:dyDescent="0.15">
@@ -6076,7 +6076,7 @@
         <v>0</v>
       </c>
       <c r="E174" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175" spans="2:5" x14ac:dyDescent="0.15">
@@ -7630,7 +7630,7 @@
         <v>0</v>
       </c>
       <c r="E285" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="286" spans="2:5" x14ac:dyDescent="0.15">
@@ -7896,7 +7896,7 @@
         <v>0</v>
       </c>
       <c r="E304" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="305" spans="2:5" x14ac:dyDescent="0.15">
@@ -7966,7 +7966,7 @@
         <v>0</v>
       </c>
       <c r="E309" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="310" spans="2:5" x14ac:dyDescent="0.15">
@@ -8792,7 +8792,7 @@
         <v>0</v>
       </c>
       <c r="E368" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="369" spans="2:5" x14ac:dyDescent="0.15">
@@ -8988,7 +8988,7 @@
         <v>0</v>
       </c>
       <c r="E382" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="383" spans="2:5" x14ac:dyDescent="0.15">
@@ -9436,7 +9436,7 @@
         <v>0</v>
       </c>
       <c r="E414" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="415" spans="2:5" x14ac:dyDescent="0.15">
@@ -9562,7 +9562,7 @@
         <v>0</v>
       </c>
       <c r="E423" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="424" spans="2:5" x14ac:dyDescent="0.15">
@@ -10626,7 +10626,7 @@
         <v>0</v>
       </c>
       <c r="E499" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="500" spans="2:5" x14ac:dyDescent="0.15">
@@ -11914,7 +11914,7 @@
         <v>0</v>
       </c>
       <c r="E591" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="592" spans="2:5" x14ac:dyDescent="0.15">
@@ -12012,7 +12012,7 @@
         <v>0</v>
       </c>
       <c r="E598" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="599" spans="2:5" x14ac:dyDescent="0.15">
@@ -12642,7 +12642,7 @@
         <v>0</v>
       </c>
       <c r="E643" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="644" spans="2:5" x14ac:dyDescent="0.15">
@@ -12894,7 +12894,7 @@
         <v>0</v>
       </c>
       <c r="E661" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="662" spans="2:5" x14ac:dyDescent="0.15">
@@ -12964,7 +12964,7 @@
         <v>1</v>
       </c>
       <c r="E666" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="667" spans="2:5" x14ac:dyDescent="0.15">
@@ -14714,7 +14714,7 @@
         <v>0</v>
       </c>
       <c r="E791" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="792" spans="2:5" x14ac:dyDescent="0.15">
@@ -15498,7 +15498,7 @@
         <v>0</v>
       </c>
       <c r="E847" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="848" spans="2:5" x14ac:dyDescent="0.15">

</xml_diff>